<commit_message>
minor edits to LFM data
saving as csv and reorganizing columns
</commit_message>
<xml_diff>
--- a/2021/LFM_WP_Fall2021/PWD_Oct2021_LFM_WP_Calcs.xlsx
+++ b/2021/LFM_WP_Fall2021/PWD_Oct2021_LFM_WP_Calcs.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melinakozanitas/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melinakozanitas/GitHub/PepperwoodVegPlots/2021/LFM_WP_Fall2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDD4294-5619-C94B-A5FE-9F0C6DA24CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00D5E19-1FB0-C248-860B-E48435061B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="460" windowWidth="27000" windowHeight="15480" activeTab="4" xr2:uid="{05CBDBC3-C58E-254F-9CCB-F423A62E9A36}"/>
+    <workbookView xWindow="1420" yWindow="460" windowWidth="27000" windowHeight="15480" activeTab="3" xr2:uid="{05CBDBC3-C58E-254F-9CCB-F423A62E9A36}"/>
   </bookViews>
   <sheets>
     <sheet name="WP_clean" sheetId="2" r:id="rId1"/>
-    <sheet name="WP_mean" sheetId="3" r:id="rId2"/>
+    <sheet name="WP_means" sheetId="3" r:id="rId2"/>
     <sheet name="LFM_clean" sheetId="1" r:id="rId3"/>
-    <sheet name="LFM_calcs" sheetId="4" r:id="rId4"/>
+    <sheet name="LFM_calcs_formulas" sheetId="4" r:id="rId4"/>
     <sheet name="FLM_final" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="119">
   <si>
     <t>Site</t>
   </si>
@@ -841,9 +841,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB63F9D-A779-474A-9790-68A1B1C3510F}">
   <dimension ref="A1:AC154"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
+    <sheetView topLeftCell="D1" zoomScale="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5695,7 +5695,7 @@
   <dimension ref="A1:K154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:C18"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7754,9 +7754,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17ACA9F-3409-0E43-A145-3AF267DD9BC7}">
   <dimension ref="A1:T143"/>
   <sheetViews>
-    <sheetView zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="K55" sqref="K55"/>
+    <sheetView zoomScale="87" zoomScaleNormal="158" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="H121" sqref="H121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8493,20 +8493,10 @@
       <c r="J30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O30" s="4">
-        <v>38.386119999999998</v>
-      </c>
+      <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
-      <c r="R30">
-        <v>39.656999999999996</v>
-      </c>
-      <c r="S30">
-        <v>37.225000000000001</v>
-      </c>
-      <c r="T30" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="T30" s="4"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -11328,8 +11318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9031B472-3627-4E45-A195-B1D10EC254E7}">
   <dimension ref="A1:V143"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11422,15 +11412,15 @@
         <v>37.119999999999997</v>
       </c>
       <c r="O2">
-        <f>(H2-N2)</f>
+        <f t="shared" ref="O2:O20" si="0">(H2-N2)</f>
         <v>1.6430000000000007</v>
       </c>
       <c r="P2">
-        <f>(E2-N2)</f>
+        <f t="shared" ref="P2:P20" si="1">(E2-N2)</f>
         <v>0.89550000000000551</v>
       </c>
       <c r="Q2">
-        <f>(O2-P2)</f>
+        <f t="shared" ref="Q2:Q33" si="2">(O2-P2)</f>
         <v>0.74749999999999517</v>
       </c>
     </row>
@@ -11460,15 +11450,15 @@
         <v>37.210999999999999</v>
       </c>
       <c r="O3">
-        <f>(H3-N3)</f>
+        <f t="shared" si="0"/>
         <v>2.4278000000000048</v>
       </c>
       <c r="P3">
-        <f>(E3-N3)</f>
+        <f t="shared" si="1"/>
         <v>1.4600000000000009</v>
       </c>
       <c r="Q3">
-        <f>(O3-P3)</f>
+        <f t="shared" si="2"/>
         <v>0.96780000000000399</v>
       </c>
     </row>
@@ -11498,15 +11488,15 @@
         <v>37.091999999999999</v>
       </c>
       <c r="O4">
-        <f>(H4-N4)</f>
+        <f t="shared" si="0"/>
         <v>2.5320000000000036</v>
       </c>
       <c r="P4">
-        <f>(E4-N4)</f>
+        <f t="shared" si="1"/>
         <v>1.4804999999999993</v>
       </c>
       <c r="Q4">
-        <f>(O4-P4)</f>
+        <f t="shared" si="2"/>
         <v>1.0515000000000043</v>
       </c>
     </row>
@@ -11536,15 +11526,15 @@
         <v>36.9848</v>
       </c>
       <c r="O5">
-        <f>(H5-N5)</f>
+        <f t="shared" si="0"/>
         <v>2.2931999999999988</v>
       </c>
       <c r="P5">
-        <f>(E5-N5)</f>
+        <f t="shared" si="1"/>
         <v>1.1328000000000031</v>
       </c>
       <c r="Q5">
-        <f>(O5-P5)</f>
+        <f t="shared" si="2"/>
         <v>1.1603999999999957</v>
       </c>
     </row>
@@ -11574,15 +11564,15 @@
         <v>36.97</v>
       </c>
       <c r="O6">
-        <f>(H6-N6)</f>
+        <f t="shared" si="0"/>
         <v>2.9442999999999984</v>
       </c>
       <c r="P6">
-        <f>(E6-N6)</f>
+        <f t="shared" si="1"/>
         <v>1.764400000000002</v>
       </c>
       <c r="Q6">
-        <f>(O6-P6)</f>
+        <f t="shared" si="2"/>
         <v>1.1798999999999964</v>
       </c>
     </row>
@@ -11612,15 +11602,15 @@
         <v>36.878</v>
       </c>
       <c r="O7">
-        <f>(H7-N7)</f>
+        <f t="shared" si="0"/>
         <v>2.6760000000000019</v>
       </c>
       <c r="P7">
-        <f>(E7-N7)</f>
+        <f t="shared" si="1"/>
         <v>1.4654000000000025</v>
       </c>
       <c r="Q7">
-        <f>(O7-P7)</f>
+        <f t="shared" si="2"/>
         <v>1.2105999999999995</v>
       </c>
     </row>
@@ -11653,15 +11643,15 @@
         <v>37.225000000000001</v>
       </c>
       <c r="O8">
-        <f>(H8-N8)</f>
+        <f t="shared" si="0"/>
         <v>2.4319999999999951</v>
       </c>
       <c r="P8">
-        <f>(E8-N8)</f>
+        <f t="shared" si="1"/>
         <v>1.1611199999999968</v>
       </c>
       <c r="Q8">
-        <f>(O8-P8)</f>
+        <f t="shared" si="2"/>
         <v>1.2708799999999982</v>
       </c>
       <c r="R8" t="s">
@@ -11695,15 +11685,15 @@
         <v>37.223999999999997</v>
       </c>
       <c r="O9">
-        <f>(H9-N9)</f>
+        <f t="shared" si="0"/>
         <v>2.7450000000000045</v>
       </c>
       <c r="P9">
-        <f>(E9-N9)</f>
+        <f t="shared" si="1"/>
         <v>1.4137000000000057</v>
       </c>
       <c r="Q9">
-        <f>(O9-P9)</f>
+        <f t="shared" si="2"/>
         <v>1.3312999999999988</v>
       </c>
     </row>
@@ -11736,15 +11726,15 @@
         <v>36.9283</v>
       </c>
       <c r="O10">
-        <f>(H10-N10)</f>
+        <f t="shared" si="0"/>
         <v>3.4956999999999994</v>
       </c>
       <c r="P10">
-        <f>(E10-N10)</f>
+        <f t="shared" si="1"/>
         <v>2.1475999999999971</v>
       </c>
       <c r="Q10">
-        <f>(O10-P10)</f>
+        <f t="shared" si="2"/>
         <v>1.3481000000000023</v>
       </c>
     </row>
@@ -11774,15 +11764,15 @@
         <v>36.988</v>
       </c>
       <c r="O11">
-        <f>(H11-N11)</f>
+        <f t="shared" si="0"/>
         <v>3.8500000000000014</v>
       </c>
       <c r="P11">
-        <f>(E11-N11)</f>
+        <f t="shared" si="1"/>
         <v>2.4579000000000022</v>
       </c>
       <c r="Q11">
-        <f>(O11-P11)</f>
+        <f t="shared" si="2"/>
         <v>1.3920999999999992</v>
       </c>
     </row>
@@ -11812,15 +11802,15 @@
         <v>37.171999999999997</v>
       </c>
       <c r="O12">
-        <f>(H12-N12)</f>
+        <f t="shared" si="0"/>
         <v>2.5450000000000017</v>
       </c>
       <c r="P12">
-        <f>(E12-N12)</f>
+        <f t="shared" si="1"/>
         <v>1.1512000000000029</v>
       </c>
       <c r="Q12">
-        <f>(O12-P12)</f>
+        <f t="shared" si="2"/>
         <v>1.3937999999999988</v>
       </c>
     </row>
@@ -11850,15 +11840,15 @@
         <v>37.024999999999999</v>
       </c>
       <c r="O13">
-        <f>(H13-N13)</f>
+        <f t="shared" si="0"/>
         <v>4.5373000000000019</v>
       </c>
       <c r="P13">
-        <f>(E13-N13)</f>
+        <f t="shared" si="1"/>
         <v>3.1405999999999992</v>
       </c>
       <c r="Q13">
-        <f>(O13-P13)</f>
+        <f t="shared" si="2"/>
         <v>1.3967000000000027</v>
       </c>
     </row>
@@ -11888,15 +11878,15 @@
         <v>37.192999999999998</v>
       </c>
       <c r="O14">
-        <f>(H14-N14)</f>
+        <f t="shared" si="0"/>
         <v>2.7110000000000056</v>
       </c>
       <c r="P14">
-        <f>(E14-N14)</f>
+        <f t="shared" si="1"/>
         <v>1.2621099999999998</v>
       </c>
       <c r="Q14">
-        <f>(O14-P14)</f>
+        <f t="shared" si="2"/>
         <v>1.4488900000000058</v>
       </c>
     </row>
@@ -11926,15 +11916,15 @@
         <v>37.023000000000003</v>
       </c>
       <c r="O15">
-        <f>(H15-N15)</f>
+        <f t="shared" si="0"/>
         <v>3.0319999999999965</v>
       </c>
       <c r="P15">
-        <f>(E15-N15)</f>
+        <f t="shared" si="1"/>
         <v>1.5504999999999995</v>
       </c>
       <c r="Q15">
-        <f>(O15-P15)</f>
+        <f t="shared" si="2"/>
         <v>1.4814999999999969</v>
       </c>
     </row>
@@ -11964,15 +11954,15 @@
         <v>37.036999999999999</v>
       </c>
       <c r="O16">
-        <f>(H16-N16)</f>
+        <f t="shared" si="0"/>
         <v>3.5850000000000009</v>
       </c>
       <c r="P16">
-        <f>(E16-N16)</f>
+        <f t="shared" si="1"/>
         <v>2.072499999999998</v>
       </c>
       <c r="Q16">
-        <f>(O16-P16)</f>
+        <f t="shared" si="2"/>
         <v>1.5125000000000028</v>
       </c>
     </row>
@@ -12002,15 +11992,15 @@
         <v>37.155000000000001</v>
       </c>
       <c r="O17">
-        <f>(H17-N17)</f>
+        <f t="shared" si="0"/>
         <v>4.2939999999999969</v>
       </c>
       <c r="P17">
-        <f>(E17-N17)</f>
+        <f t="shared" si="1"/>
         <v>2.7160000000000011</v>
       </c>
       <c r="Q17">
-        <f>(O17-P17)</f>
+        <f t="shared" si="2"/>
         <v>1.5779999999999959</v>
       </c>
     </row>
@@ -12040,15 +12030,15 @@
         <v>37.020000000000003</v>
       </c>
       <c r="O18">
-        <f>(H18-N18)</f>
+        <f t="shared" si="0"/>
         <v>4.4649999999999963</v>
       </c>
       <c r="P18">
-        <f>(E18-N18)</f>
+        <f t="shared" si="1"/>
         <v>2.8741999999999948</v>
       </c>
       <c r="Q18">
-        <f>(O18-P18)</f>
+        <f t="shared" si="2"/>
         <v>1.5908000000000015</v>
       </c>
     </row>
@@ -12078,15 +12068,15 @@
         <v>37.134</v>
       </c>
       <c r="O19">
-        <f>(H19-N19)</f>
+        <f t="shared" si="0"/>
         <v>4.4572999999999965</v>
       </c>
       <c r="P19">
-        <f>(E19-N19)</f>
+        <f t="shared" si="1"/>
         <v>2.8494000000000028</v>
       </c>
       <c r="Q19">
-        <f>(O19-P19)</f>
+        <f t="shared" si="2"/>
         <v>1.6078999999999937</v>
       </c>
     </row>
@@ -12116,15 +12106,15 @@
         <v>37.045999999999999</v>
       </c>
       <c r="O20">
-        <f>(H20-N20)</f>
+        <f t="shared" si="0"/>
         <v>3.2250000000000014</v>
       </c>
       <c r="P20">
-        <f>(E20-N20)</f>
+        <f t="shared" si="1"/>
         <v>1.5636999999999972</v>
       </c>
       <c r="Q20">
-        <f>(O20-P20)</f>
+        <f t="shared" si="2"/>
         <v>1.6613000000000042</v>
       </c>
     </row>
@@ -12175,7 +12165,7 @@
         <v>1.6618500000000012</v>
       </c>
       <c r="Q21">
-        <f>(O21-P21)</f>
+        <f t="shared" si="2"/>
         <v>1.7111499999999964</v>
       </c>
       <c r="R21" t="s">
@@ -12208,15 +12198,15 @@
         <v>37.076000000000001</v>
       </c>
       <c r="O22">
-        <f>(H22-N22)</f>
+        <f t="shared" ref="O22:O30" si="3">(H22-N22)</f>
         <v>4.527000000000001</v>
       </c>
       <c r="P22">
-        <f>(E22-N22)</f>
+        <f t="shared" ref="P22:P30" si="4">(E22-N22)</f>
         <v>2.7622999999999962</v>
       </c>
       <c r="Q22">
-        <f>(O22-P22)</f>
+        <f t="shared" si="2"/>
         <v>1.7647000000000048</v>
       </c>
     </row>
@@ -12246,15 +12236,15 @@
         <v>37.106000000000002</v>
       </c>
       <c r="O23">
-        <f>(H23-N23)</f>
+        <f t="shared" si="3"/>
         <v>3.205999999999996</v>
       </c>
       <c r="P23">
-        <f>(E23-N23)</f>
+        <f t="shared" si="4"/>
         <v>1.3618799999999993</v>
       </c>
       <c r="Q23">
-        <f>(O23-P23)</f>
+        <f t="shared" si="2"/>
         <v>1.8441199999999967</v>
       </c>
     </row>
@@ -12284,15 +12274,15 @@
         <v>37.067</v>
       </c>
       <c r="O24">
-        <f>(H24-N24)</f>
+        <f t="shared" si="3"/>
         <v>4.8830000000000027</v>
       </c>
       <c r="P24">
-        <f>(E24-N24)</f>
+        <f t="shared" si="4"/>
         <v>3.0150999999999968</v>
       </c>
       <c r="Q24">
-        <f>(O24-P24)</f>
+        <f t="shared" si="2"/>
         <v>1.8679000000000059</v>
       </c>
     </row>
@@ -12322,15 +12312,15 @@
         <v>37.101999999999997</v>
       </c>
       <c r="O25">
-        <f>(H25-N25)</f>
+        <f t="shared" si="3"/>
         <v>4.7244000000000028</v>
       </c>
       <c r="P25">
-        <f>(E25-N25)</f>
+        <f t="shared" si="4"/>
         <v>2.8198000000000008</v>
       </c>
       <c r="Q25">
-        <f>(O25-P25)</f>
+        <f t="shared" si="2"/>
         <v>1.9046000000000021</v>
       </c>
     </row>
@@ -12360,15 +12350,15 @@
         <v>37.088000000000001</v>
       </c>
       <c r="O26">
-        <f>(H26-N26)</f>
+        <f t="shared" si="3"/>
         <v>5.6077000000000012</v>
       </c>
       <c r="P26">
-        <f>(E26-N26)</f>
+        <f t="shared" si="4"/>
         <v>3.693799999999996</v>
       </c>
       <c r="Q26">
-        <f>(O26-P26)</f>
+        <f t="shared" si="2"/>
         <v>1.9139000000000053</v>
       </c>
     </row>
@@ -12398,15 +12388,15 @@
         <v>36.860999999999997</v>
       </c>
       <c r="O27">
-        <f>(H27-N27)</f>
+        <f t="shared" si="3"/>
         <v>3.7439999999999998</v>
       </c>
       <c r="P27">
-        <f>(E27-N27)</f>
+        <f t="shared" si="4"/>
         <v>1.8231999999999999</v>
       </c>
       <c r="Q27">
-        <f>(O27-P27)</f>
+        <f t="shared" si="2"/>
         <v>1.9207999999999998</v>
       </c>
     </row>
@@ -12436,15 +12426,15 @@
         <v>37.135599999999997</v>
       </c>
       <c r="O28">
-        <f>(H28-N28)</f>
+        <f t="shared" si="3"/>
         <v>5.0025000000000048</v>
       </c>
       <c r="P28">
-        <f>(E28-N28)</f>
+        <f t="shared" si="4"/>
         <v>3.0777000000000001</v>
       </c>
       <c r="Q28">
-        <f>(O28-P28)</f>
+        <f t="shared" si="2"/>
         <v>1.9248000000000047</v>
       </c>
     </row>
@@ -12475,15 +12465,15 @@
         <v>37.121000000000002</v>
       </c>
       <c r="O29">
-        <f>(H29-N29)</f>
+        <f t="shared" si="3"/>
         <v>2.8109999999999999</v>
       </c>
       <c r="P29">
-        <f>(E29-N29)</f>
+        <f t="shared" si="4"/>
         <v>0.87930000000000064</v>
       </c>
       <c r="Q29">
-        <f>(O29-P29)</f>
+        <f t="shared" si="2"/>
         <v>1.9316999999999993</v>
       </c>
     </row>
@@ -12513,15 +12503,15 @@
         <v>36.911999999999999</v>
       </c>
       <c r="O30">
-        <f>(H30-N30)</f>
+        <f t="shared" si="3"/>
         <v>4.7150000000000034</v>
       </c>
       <c r="P30">
-        <f>(E30-N30)</f>
+        <f t="shared" si="4"/>
         <v>2.7801000000000045</v>
       </c>
       <c r="Q30">
-        <f>(O30-P30)</f>
+        <f t="shared" si="2"/>
         <v>1.934899999999999</v>
       </c>
     </row>
@@ -12569,7 +12559,7 @@
         <v>2.3389999999999986</v>
       </c>
       <c r="Q31">
-        <f>(O31-P31)</f>
+        <f t="shared" si="2"/>
         <v>1.9579999999999984</v>
       </c>
     </row>
@@ -12607,7 +12597,7 @@
         <v>1.9758999999999958</v>
       </c>
       <c r="Q32">
-        <f>(O32-P32)</f>
+        <f t="shared" si="2"/>
         <v>1.9761000000000024</v>
       </c>
     </row>
@@ -12645,7 +12635,7 @@
         <v>3.6576999999999984</v>
       </c>
       <c r="Q33">
-        <f>(O33-P33)</f>
+        <f t="shared" si="2"/>
         <v>2.0763000000000034</v>
       </c>
     </row>
@@ -12683,7 +12673,7 @@
         <v>3.0686999999999998</v>
       </c>
       <c r="Q34">
-        <f>(O34-P34)</f>
+        <f t="shared" ref="Q34:Q65" si="5">(O34-P34)</f>
         <v>2.2130999999999972</v>
       </c>
     </row>
@@ -12721,7 +12711,7 @@
         <v>2.8061999999999969</v>
       </c>
       <c r="Q35">
-        <f>(O35-P35)</f>
+        <f t="shared" si="5"/>
         <v>2.2206000000000046</v>
       </c>
     </row>
@@ -12769,7 +12759,7 @@
         <v>2.1353000000000009</v>
       </c>
       <c r="Q36">
-        <f>(O36-P36)</f>
+        <f t="shared" si="5"/>
         <v>2.2316999999999965</v>
       </c>
     </row>
@@ -12807,7 +12797,7 @@
         <v>3.6137999999999977</v>
       </c>
       <c r="Q37">
-        <f>(O37-P37)</f>
+        <f t="shared" si="5"/>
         <v>2.4282000000000039</v>
       </c>
     </row>
@@ -12845,7 +12835,7 @@
         <v>3.5564999999999998</v>
       </c>
       <c r="Q38">
-        <f>(O38-P38)</f>
+        <f t="shared" si="5"/>
         <v>2.4354999999999976</v>
       </c>
     </row>
@@ -12883,7 +12873,7 @@
         <v>3.9873999999999938</v>
       </c>
       <c r="Q39">
-        <f>(O39-P39)</f>
+        <f t="shared" si="5"/>
         <v>2.5086000000000013</v>
       </c>
     </row>
@@ -12928,7 +12918,7 @@
         <v>4.5165999999999968</v>
       </c>
       <c r="Q40">
-        <f>(O40-P40)</f>
+        <f t="shared" si="5"/>
         <v>2.5804000000000045</v>
       </c>
       <c r="R40" t="s">
@@ -12979,7 +12969,7 @@
         <v>4.3102799999999988</v>
       </c>
       <c r="Q41">
-        <f>(O41-P41)</f>
+        <f t="shared" si="5"/>
         <v>2.6617200000000025</v>
       </c>
       <c r="R41" t="s">
@@ -13012,15 +13002,15 @@
         <v>37.085999999999999</v>
       </c>
       <c r="O42">
-        <f>(H42-N42)</f>
+        <f t="shared" ref="O42:O49" si="6">(H42-N42)</f>
         <v>6.9909999999999997</v>
       </c>
       <c r="P42">
-        <f>(E42-N42)</f>
+        <f t="shared" ref="P42:P49" si="7">(E42-N42)</f>
         <v>4.2635000000000005</v>
       </c>
       <c r="Q42">
-        <f>(O42-P42)</f>
+        <f t="shared" si="5"/>
         <v>2.7274999999999991</v>
       </c>
     </row>
@@ -13050,15 +13040,15 @@
         <v>37.161000000000001</v>
       </c>
       <c r="O43">
-        <f>(H43-N43)</f>
+        <f t="shared" si="6"/>
         <v>5.4110000000000014</v>
       </c>
       <c r="P43">
-        <f>(E43-N43)</f>
+        <f t="shared" si="7"/>
         <v>2.6822999999999979</v>
       </c>
       <c r="Q43">
-        <f>(O43-P43)</f>
+        <f t="shared" si="5"/>
         <v>2.7287000000000035</v>
       </c>
     </row>
@@ -13088,15 +13078,15 @@
         <v>37.005000000000003</v>
       </c>
       <c r="O44">
-        <f>(H44-N44)</f>
+        <f t="shared" si="6"/>
         <v>5.6175999999999959</v>
       </c>
       <c r="P44">
-        <f>(E44-N44)</f>
+        <f t="shared" si="7"/>
         <v>2.7937999999999974</v>
       </c>
       <c r="Q44">
-        <f>(O44-P44)</f>
+        <f t="shared" si="5"/>
         <v>2.8237999999999985</v>
       </c>
     </row>
@@ -13126,15 +13116,15 @@
         <v>37.056399999999996</v>
       </c>
       <c r="O45">
-        <f>(H45-N45)</f>
+        <f t="shared" si="6"/>
         <v>7.2052000000000049</v>
       </c>
       <c r="P45">
-        <f>(E45-N45)</f>
+        <f t="shared" si="7"/>
         <v>4.3102000000000018</v>
       </c>
       <c r="Q45">
-        <f>(O45-P45)</f>
+        <f t="shared" si="5"/>
         <v>2.8950000000000031</v>
       </c>
     </row>
@@ -13167,15 +13157,15 @@
         <v>37.084000000000003</v>
       </c>
       <c r="O46">
-        <f>(H46-N46)</f>
+        <f t="shared" si="6"/>
         <v>7.4259999999999948</v>
       </c>
       <c r="P46">
-        <f>(E46-N46)</f>
+        <f t="shared" si="7"/>
         <v>4.4739999999999966</v>
       </c>
       <c r="Q46">
-        <f>(O46-P46)</f>
+        <f t="shared" si="5"/>
         <v>2.9519999999999982</v>
       </c>
     </row>
@@ -13205,15 +13195,15 @@
         <v>37.136000000000003</v>
       </c>
       <c r="O47">
-        <f>(H47-N47)</f>
+        <f t="shared" si="6"/>
         <v>6.7409999999999997</v>
       </c>
       <c r="P47">
-        <f>(E47-N47)</f>
+        <f t="shared" si="7"/>
         <v>3.746699999999997</v>
       </c>
       <c r="Q47">
-        <f>(O47-P47)</f>
+        <f t="shared" si="5"/>
         <v>2.9943000000000026</v>
       </c>
     </row>
@@ -13243,15 +13233,15 @@
         <v>37.006999999999998</v>
       </c>
       <c r="O48">
-        <f>(H48-N48)</f>
+        <f t="shared" si="6"/>
         <v>8.7220000000000013</v>
       </c>
       <c r="P48">
-        <f>(E48-N48)</f>
+        <f t="shared" si="7"/>
         <v>5.7161000000000044</v>
       </c>
       <c r="Q48">
-        <f>(O48-P48)</f>
+        <f t="shared" si="5"/>
         <v>3.0058999999999969</v>
       </c>
       <c r="V48" s="10"/>
@@ -13282,15 +13272,15 @@
         <v>36.899799999999999</v>
       </c>
       <c r="O49">
-        <f>(H49-N49)</f>
+        <f t="shared" si="6"/>
         <v>6.9234000000000009</v>
       </c>
       <c r="P49">
-        <f>(E49-N49)</f>
+        <f t="shared" si="7"/>
         <v>3.8387999999999991</v>
       </c>
       <c r="Q49">
-        <f>(O49-P49)</f>
+        <f t="shared" si="5"/>
         <v>3.0846000000000018</v>
       </c>
     </row>
@@ -13338,7 +13328,7 @@
         <v>6.5616000000000057</v>
       </c>
       <c r="Q50">
-        <f>(O50-P50)</f>
+        <f t="shared" si="5"/>
         <v>3.1933999999999969</v>
       </c>
       <c r="R50" t="s">
@@ -13377,15 +13367,15 @@
         <v>37.145000000000003</v>
       </c>
       <c r="O51">
-        <f>(H51-N51)</f>
+        <f t="shared" ref="O51:O95" si="8">(H51-N51)</f>
         <v>9.3739999999999952</v>
       </c>
       <c r="P51">
-        <f>(E51-N51)</f>
+        <f t="shared" ref="P51:P95" si="9">(E51-N51)</f>
         <v>6.1538799999999938</v>
       </c>
       <c r="Q51">
-        <f>(O51-P51)</f>
+        <f t="shared" si="5"/>
         <v>3.2201200000000014</v>
       </c>
     </row>
@@ -13415,15 +13405,15 @@
         <v>36.951999999999998</v>
       </c>
       <c r="O52">
-        <f>(H52-N52)</f>
+        <f t="shared" si="8"/>
         <v>9.0100000000000051</v>
       </c>
       <c r="P52">
-        <f>(E52-N52)</f>
+        <f t="shared" si="9"/>
         <v>5.7886000000000024</v>
       </c>
       <c r="Q52">
-        <f>(O52-P52)</f>
+        <f t="shared" si="5"/>
         <v>3.2214000000000027</v>
       </c>
     </row>
@@ -13453,15 +13443,15 @@
         <v>37.011899999999997</v>
       </c>
       <c r="O53">
-        <f>(H53-N53)</f>
+        <f t="shared" si="8"/>
         <v>8.3719999999999999</v>
       </c>
       <c r="P53">
-        <f>(E53-N53)</f>
+        <f t="shared" si="9"/>
         <v>5.0400000000000063</v>
       </c>
       <c r="Q53">
-        <f>(O53-P53)</f>
+        <f t="shared" si="5"/>
         <v>3.3319999999999936</v>
       </c>
     </row>
@@ -13491,15 +13481,15 @@
         <v>36.976100000000002</v>
       </c>
       <c r="O54">
-        <f>(H54-N54)</f>
+        <f t="shared" si="8"/>
         <v>8.1861999999999995</v>
       </c>
       <c r="P54">
-        <f>(E54-N54)</f>
+        <f t="shared" si="9"/>
         <v>4.8125999999999962</v>
       </c>
       <c r="Q54">
-        <f>(O54-P54)</f>
+        <f t="shared" si="5"/>
         <v>3.3736000000000033</v>
       </c>
     </row>
@@ -13529,15 +13519,15 @@
         <v>37.134999999999998</v>
       </c>
       <c r="O55">
-        <f>(H55-N55)</f>
+        <f t="shared" si="8"/>
         <v>9.1340000000000003</v>
       </c>
       <c r="P55">
-        <f>(E55-N55)</f>
+        <f t="shared" si="9"/>
         <v>5.7446000000000055</v>
       </c>
       <c r="Q55">
-        <f>(O55-P55)</f>
+        <f t="shared" si="5"/>
         <v>3.3893999999999949</v>
       </c>
     </row>
@@ -13567,15 +13557,15 @@
         <v>37.017899999999997</v>
       </c>
       <c r="O56">
-        <f>(H56-N56)</f>
+        <f t="shared" si="8"/>
         <v>7.8845000000000027</v>
       </c>
       <c r="P56">
-        <f>(E56-N56)</f>
+        <f t="shared" si="9"/>
         <v>4.4747000000000057</v>
       </c>
       <c r="Q56">
-        <f>(O56-P56)</f>
+        <f t="shared" si="5"/>
         <v>3.4097999999999971</v>
       </c>
     </row>
@@ -13605,15 +13595,15 @@
         <v>37.130000000000003</v>
       </c>
       <c r="O57">
-        <f>(H57-N57)</f>
+        <f t="shared" si="8"/>
         <v>6.5229999999999961</v>
       </c>
       <c r="P57">
-        <f>(E57-N57)</f>
+        <f t="shared" si="9"/>
         <v>3.0805000000000007</v>
       </c>
       <c r="Q57">
-        <f>(O57-P57)</f>
+        <f t="shared" si="5"/>
         <v>3.4424999999999955</v>
       </c>
     </row>
@@ -13646,15 +13636,15 @@
         <v>37.015000000000001</v>
       </c>
       <c r="O58">
-        <f>(H58-N58)</f>
+        <f t="shared" si="8"/>
         <v>6.3190000000000026</v>
       </c>
       <c r="P58">
-        <f>(E58-N58)</f>
+        <f t="shared" si="9"/>
         <v>2.8699099999999973</v>
       </c>
       <c r="Q58">
-        <f>(O58-P58)</f>
+        <f t="shared" si="5"/>
         <v>3.4490900000000053</v>
       </c>
       <c r="R58" t="s">
@@ -13687,15 +13677,15 @@
         <v>36.878999999999998</v>
       </c>
       <c r="O59">
-        <f>(H59-N59)</f>
+        <f t="shared" si="8"/>
         <v>7.0600000000000023</v>
       </c>
       <c r="P59">
-        <f>(E59-N59)</f>
+        <f t="shared" si="9"/>
         <v>3.5777300000000025</v>
       </c>
       <c r="Q59">
-        <f>(O59-P59)</f>
+        <f t="shared" si="5"/>
         <v>3.4822699999999998</v>
       </c>
     </row>
@@ -13725,15 +13715,15 @@
         <v>37.198999999999998</v>
       </c>
       <c r="O60">
-        <f>(H60-N60)</f>
+        <f t="shared" si="8"/>
         <v>6.9879000000000033</v>
       </c>
       <c r="P60">
-        <f>(E60-N60)</f>
+        <f t="shared" si="9"/>
         <v>3.4220000000000041</v>
       </c>
       <c r="Q60">
-        <f>(O60-P60)</f>
+        <f t="shared" si="5"/>
         <v>3.5658999999999992</v>
       </c>
     </row>
@@ -13763,15 +13753,15 @@
         <v>37.005000000000003</v>
       </c>
       <c r="O61">
-        <f>(H61-N61)</f>
+        <f t="shared" si="8"/>
         <v>6.5210000000000008</v>
       </c>
       <c r="P61">
-        <f>(E61-N61)</f>
+        <f t="shared" si="9"/>
         <v>2.8845999999999989</v>
       </c>
       <c r="Q61">
-        <f>(O61-P61)</f>
+        <f t="shared" si="5"/>
         <v>3.6364000000000019</v>
       </c>
     </row>
@@ -13801,15 +13791,15 @@
         <v>37.155000000000001</v>
       </c>
       <c r="O62">
-        <f>(H62-N62)</f>
+        <f t="shared" si="8"/>
         <v>9.8489999999999966</v>
       </c>
       <c r="P62">
-        <f>(E62-N62)</f>
+        <f t="shared" si="9"/>
         <v>6.1597999999999971</v>
       </c>
       <c r="Q62">
-        <f>(O62-P62)</f>
+        <f t="shared" si="5"/>
         <v>3.6891999999999996</v>
       </c>
     </row>
@@ -13839,15 +13829,15 @@
         <v>36.954000000000001</v>
       </c>
       <c r="O63">
-        <f>(H63-N63)</f>
+        <f t="shared" si="8"/>
         <v>7.5779999999999959</v>
       </c>
       <c r="P63">
-        <f>(E63-N63)</f>
+        <f t="shared" si="9"/>
         <v>3.8476900000000001</v>
       </c>
       <c r="Q63">
-        <f>(O63-P63)</f>
+        <f t="shared" si="5"/>
         <v>3.7303099999999958</v>
       </c>
     </row>
@@ -13877,15 +13867,15 @@
         <v>37.110399999999998</v>
       </c>
       <c r="O64">
-        <f>(H64-N64)</f>
+        <f t="shared" si="8"/>
         <v>8.6373000000000033</v>
       </c>
       <c r="P64">
-        <f>(E64-N64)</f>
+        <f t="shared" si="9"/>
         <v>4.9040999999999997</v>
       </c>
       <c r="Q64">
-        <f>(O64-P64)</f>
+        <f t="shared" si="5"/>
         <v>3.7332000000000036</v>
       </c>
     </row>
@@ -13915,15 +13905,15 @@
         <v>37.018900000000002</v>
       </c>
       <c r="O65">
-        <f>(H65-N65)</f>
+        <f t="shared" si="8"/>
         <v>9.6395999999999944</v>
       </c>
       <c r="P65">
-        <f>(E65-N65)</f>
+        <f t="shared" si="9"/>
         <v>5.7680000000000007</v>
       </c>
       <c r="Q65">
-        <f>(O65-P65)</f>
+        <f t="shared" si="5"/>
         <v>3.8715999999999937</v>
       </c>
     </row>
@@ -13953,15 +13943,15 @@
         <v>37.155999999999999</v>
       </c>
       <c r="O66">
-        <f>(H66-N66)</f>
+        <f t="shared" si="8"/>
         <v>9.2049999999999983</v>
       </c>
       <c r="P66">
-        <f>(E66-N66)</f>
+        <f t="shared" si="9"/>
         <v>5.1688000000000045</v>
       </c>
       <c r="Q66">
-        <f>(O66-P66)</f>
+        <f t="shared" ref="Q66:Q97" si="10">(O66-P66)</f>
         <v>4.0361999999999938</v>
       </c>
     </row>
@@ -13991,15 +13981,15 @@
         <v>37.058300000000003</v>
       </c>
       <c r="O67">
-        <f>(H67-N67)</f>
+        <f t="shared" si="8"/>
         <v>10.1492</v>
       </c>
       <c r="P67">
-        <f>(E67-N67)</f>
+        <f t="shared" si="9"/>
         <v>5.8194999999999979</v>
       </c>
       <c r="Q67">
-        <f>(O67-P67)</f>
+        <f t="shared" si="10"/>
         <v>4.3297000000000025</v>
       </c>
     </row>
@@ -14029,15 +14019,15 @@
         <v>37.015000000000001</v>
       </c>
       <c r="O68">
-        <f>(H68-N68)</f>
+        <f t="shared" si="8"/>
         <v>9.8113000000000028</v>
       </c>
       <c r="P68">
-        <f>(E68-N68)</f>
+        <f t="shared" si="9"/>
         <v>5.0634000000000015</v>
       </c>
       <c r="Q68">
-        <f>(O68-P68)</f>
+        <f t="shared" si="10"/>
         <v>4.7479000000000013</v>
       </c>
     </row>
@@ -14067,15 +14057,15 @@
         <v>37.084000000000003</v>
       </c>
       <c r="O69">
-        <f>(H69-N69)</f>
+        <f t="shared" si="8"/>
         <v>8.7249999999999943</v>
       </c>
       <c r="P69">
-        <f>(E69-N69)</f>
+        <f t="shared" si="9"/>
         <v>3.9636999999999958</v>
       </c>
       <c r="Q69">
-        <f>(O69-P69)</f>
+        <f t="shared" si="10"/>
         <v>4.7612999999999985</v>
       </c>
     </row>
@@ -14105,15 +14095,15 @@
         <v>37.037999999999997</v>
       </c>
       <c r="O70">
-        <f>(H70-N70)</f>
+        <f t="shared" si="8"/>
         <v>11.701000000000001</v>
       </c>
       <c r="P70">
-        <f>(E70-N70)</f>
+        <f t="shared" si="9"/>
         <v>6.6767000000000039</v>
       </c>
       <c r="Q70">
-        <f>(O70-P70)</f>
+        <f t="shared" si="10"/>
         <v>5.0242999999999967</v>
       </c>
       <c r="V70" s="10"/>
@@ -14144,15 +14134,15 @@
         <v>37.177999999999997</v>
       </c>
       <c r="O71">
-        <f>(H71-N71)</f>
+        <f t="shared" si="8"/>
         <v>13.682500000000005</v>
       </c>
       <c r="P71">
-        <f>(E71-N71)</f>
+        <f t="shared" si="9"/>
         <v>8.5907000000000053</v>
       </c>
       <c r="Q71">
-        <f>(O71-P71)</f>
+        <f t="shared" si="10"/>
         <v>5.0917999999999992</v>
       </c>
     </row>
@@ -14182,15 +14172,15 @@
         <v>37.064999999999998</v>
       </c>
       <c r="O72">
-        <f>(H72-N72)</f>
+        <f t="shared" si="8"/>
         <v>11.066000000000003</v>
       </c>
       <c r="P72">
-        <f>(E72-N72)</f>
+        <f t="shared" si="9"/>
         <v>5.940100000000001</v>
       </c>
       <c r="Q72">
-        <f>(O72-P72)</f>
+        <f t="shared" si="10"/>
         <v>5.1259000000000015</v>
       </c>
     </row>
@@ -14220,15 +14210,15 @@
         <v>36.989199999999997</v>
       </c>
       <c r="O73">
-        <f>(H73-N73)</f>
+        <f t="shared" si="8"/>
         <v>12.913800000000002</v>
       </c>
       <c r="P73">
-        <f>(E73-N73)</f>
+        <f t="shared" si="9"/>
         <v>7.4313000000000002</v>
       </c>
       <c r="Q73">
-        <f>(O73-P73)</f>
+        <f t="shared" si="10"/>
         <v>5.4825000000000017</v>
       </c>
     </row>
@@ -14261,15 +14251,15 @@
         <v>36.984699999999997</v>
       </c>
       <c r="O74">
-        <f>(H74-N74)</f>
+        <f t="shared" si="8"/>
         <v>12.778300000000002</v>
       </c>
       <c r="P74">
-        <f>(E74-N74)</f>
+        <f t="shared" si="9"/>
         <v>7.1736000000000004</v>
       </c>
       <c r="Q74">
-        <f>(O74-P74)</f>
+        <f t="shared" si="10"/>
         <v>5.6047000000000011</v>
       </c>
     </row>
@@ -14299,15 +14289,15 @@
         <v>37.131999999999998</v>
       </c>
       <c r="O75">
-        <f>(H75-N75)</f>
+        <f t="shared" si="8"/>
         <v>15.6967</v>
       </c>
       <c r="P75">
-        <f>(E75-N75)</f>
+        <f t="shared" si="9"/>
         <v>10.066800000000001</v>
       </c>
       <c r="Q75">
-        <f>(O75-P75)</f>
+        <f t="shared" si="10"/>
         <v>5.6298999999999992</v>
       </c>
     </row>
@@ -14340,15 +14330,15 @@
         <v>36.938000000000002</v>
       </c>
       <c r="O76">
-        <f>(H76-N76)</f>
+        <f t="shared" si="8"/>
         <v>14.488</v>
       </c>
       <c r="P76">
-        <f>(E76-N76)</f>
+        <f t="shared" si="9"/>
         <v>8.8297600000000003</v>
       </c>
       <c r="Q76">
-        <f>(O76-P76)</f>
+        <f t="shared" si="10"/>
         <v>5.6582399999999993</v>
       </c>
       <c r="R76" t="s">
@@ -14381,15 +14371,15 @@
         <v>31.1904</v>
       </c>
       <c r="O77">
-        <f>(H77-N77)</f>
+        <f t="shared" si="8"/>
         <v>19.072599999999998</v>
       </c>
       <c r="P77">
-        <f>(E77-N77)</f>
+        <f t="shared" si="9"/>
         <v>13.373200000000001</v>
       </c>
       <c r="Q77">
-        <f>(O77-P77)</f>
+        <f t="shared" si="10"/>
         <v>5.6993999999999971</v>
       </c>
     </row>
@@ -14422,15 +14412,15 @@
         <v>37.137099999999997</v>
       </c>
       <c r="O78">
-        <f>(H78-N78)</f>
+        <f t="shared" si="8"/>
         <v>15.528500000000001</v>
       </c>
       <c r="P78">
-        <f>(E78-N78)</f>
+        <f t="shared" si="9"/>
         <v>9.801400000000001</v>
       </c>
       <c r="Q78">
-        <f>(O78-P78)</f>
+        <f t="shared" si="10"/>
         <v>5.7271000000000001</v>
       </c>
     </row>
@@ -14462,15 +14452,15 @@
         <v>37.018500000000003</v>
       </c>
       <c r="O79">
-        <f>(H79-N79)</f>
+        <f t="shared" si="8"/>
         <v>10.536499999999997</v>
       </c>
       <c r="P79">
-        <f>(E79-N79)</f>
+        <f t="shared" si="9"/>
         <v>4.6252999999999957</v>
       </c>
       <c r="Q79">
-        <f>(O79-P79)</f>
+        <f t="shared" si="10"/>
         <v>5.9112000000000009</v>
       </c>
     </row>
@@ -14503,15 +14493,15 @@
         <v>36.9529</v>
       </c>
       <c r="O80">
-        <f>(H80-N80)</f>
+        <f t="shared" si="8"/>
         <v>13.625100000000003</v>
       </c>
       <c r="P80">
-        <f>(E80-N80)</f>
+        <f t="shared" si="9"/>
         <v>7.7109999999999985</v>
       </c>
       <c r="Q80">
-        <f>(O80-P80)</f>
+        <f t="shared" si="10"/>
         <v>5.9141000000000048</v>
       </c>
     </row>
@@ -14541,15 +14531,15 @@
         <v>36.942999999999998</v>
       </c>
       <c r="O81">
-        <f>(H81-N81)</f>
+        <f t="shared" si="8"/>
         <v>14.620000000000005</v>
       </c>
       <c r="P81">
-        <f>(E81-N81)</f>
+        <f t="shared" si="9"/>
         <v>8.6524000000000001</v>
       </c>
       <c r="Q81">
-        <f>(O81-P81)</f>
+        <f t="shared" si="10"/>
         <v>5.9676000000000045</v>
       </c>
     </row>
@@ -14579,15 +14569,15 @@
         <v>37.1113</v>
       </c>
       <c r="O82">
-        <f>(H82-N82)</f>
+        <f t="shared" si="8"/>
         <v>13.892800000000001</v>
       </c>
       <c r="P82">
-        <f>(E82-N82)</f>
+        <f t="shared" si="9"/>
         <v>7.9146000000000001</v>
       </c>
       <c r="Q82">
-        <f>(O82-P82)</f>
+        <f t="shared" si="10"/>
         <v>5.9782000000000011</v>
       </c>
     </row>
@@ -14617,15 +14607,15 @@
         <v>36.912999999999997</v>
       </c>
       <c r="O83">
-        <f>(H83-N83)</f>
+        <f t="shared" si="8"/>
         <v>14.747</v>
       </c>
       <c r="P83">
-        <f>(E83-N83)</f>
+        <f t="shared" si="9"/>
         <v>8.6831000000000031</v>
       </c>
       <c r="Q83">
-        <f>(O83-P83)</f>
+        <f t="shared" si="10"/>
         <v>6.0638999999999967</v>
       </c>
     </row>
@@ -14655,15 +14645,15 @@
         <v>37.043900000000001</v>
       </c>
       <c r="O84">
-        <f>(H84-N84)</f>
+        <f t="shared" si="8"/>
         <v>13.033099999999997</v>
       </c>
       <c r="P84">
-        <f>(E84-N84)</f>
+        <f t="shared" si="9"/>
         <v>6.816200000000002</v>
       </c>
       <c r="Q84">
-        <f>(O84-P84)</f>
+        <f t="shared" si="10"/>
         <v>6.2168999999999954</v>
       </c>
     </row>
@@ -14696,15 +14686,15 @@
         <v>37.161999999999999</v>
       </c>
       <c r="O85">
-        <f>(H85-N85)</f>
+        <f t="shared" si="8"/>
         <v>16.548999999999999</v>
       </c>
       <c r="P85">
-        <f>(E85-N85)</f>
+        <f t="shared" si="9"/>
         <v>10.255490000000002</v>
       </c>
       <c r="Q85">
-        <f>(O85-P85)</f>
+        <f t="shared" si="10"/>
         <v>6.2935099999999977</v>
       </c>
       <c r="R85" t="s">
@@ -14737,15 +14727,15 @@
         <v>37.136699999999998</v>
       </c>
       <c r="O86">
-        <f>(H86-N86)</f>
+        <f t="shared" si="8"/>
         <v>15.999300000000005</v>
       </c>
       <c r="P86">
-        <f>(E86-N86)</f>
+        <f t="shared" si="9"/>
         <v>8.6682000000000059</v>
       </c>
       <c r="Q86">
-        <f>(O86-P86)</f>
+        <f t="shared" si="10"/>
         <v>7.3310999999999993</v>
       </c>
     </row>
@@ -14775,15 +14765,15 @@
         <v>36.8932</v>
       </c>
       <c r="O87">
-        <f>(H87-N87)</f>
+        <f t="shared" si="8"/>
         <v>17.0105</v>
       </c>
       <c r="P87">
-        <f>(E87-N87)</f>
+        <f t="shared" si="9"/>
         <v>9.6546999999999983</v>
       </c>
       <c r="Q87">
-        <f>(O87-P87)</f>
+        <f t="shared" si="10"/>
         <v>7.3558000000000021</v>
       </c>
     </row>
@@ -14813,15 +14803,15 @@
         <v>37.059199999999997</v>
       </c>
       <c r="O88">
-        <f>(H88-N88)</f>
+        <f t="shared" si="8"/>
         <v>15.778800000000004</v>
       </c>
       <c r="P88">
-        <f>(E88-N88)</f>
+        <f t="shared" si="9"/>
         <v>8.3870000000000005</v>
       </c>
       <c r="Q88">
-        <f>(O88-P88)</f>
+        <f t="shared" si="10"/>
         <v>7.3918000000000035</v>
       </c>
     </row>
@@ -14857,15 +14847,15 @@
         <v>37.11</v>
       </c>
       <c r="O89">
-        <f>(H89-N89)</f>
+        <f t="shared" si="8"/>
         <v>14.203000000000003</v>
       </c>
       <c r="P89">
-        <f>(E89-N89)</f>
+        <f t="shared" si="9"/>
         <v>6.8108599999999981</v>
       </c>
       <c r="Q89">
-        <f>(O89-P89)</f>
+        <f t="shared" si="10"/>
         <v>7.3921400000000048</v>
       </c>
       <c r="R89" t="s">
@@ -14898,15 +14888,15 @@
         <v>36.857999999999997</v>
       </c>
       <c r="O90">
-        <f>(H90-N90)</f>
+        <f t="shared" si="8"/>
         <v>19.075000000000003</v>
       </c>
       <c r="P90">
-        <f>(E90-N90)</f>
+        <f t="shared" si="9"/>
         <v>11.661500000000004</v>
       </c>
       <c r="Q90">
-        <f>(O90-P90)</f>
+        <f t="shared" si="10"/>
         <v>7.4134999999999991</v>
       </c>
     </row>
@@ -14936,15 +14926,15 @@
         <v>37.017000000000003</v>
       </c>
       <c r="O91">
-        <f>(H91-N91)</f>
+        <f t="shared" si="8"/>
         <v>16.787999999999997</v>
       </c>
       <c r="P91">
-        <f>(E91-N91)</f>
+        <f t="shared" si="9"/>
         <v>9.1850499999999968</v>
       </c>
       <c r="Q91">
-        <f>(O91-P91)</f>
+        <f t="shared" si="10"/>
         <v>7.6029499999999999</v>
       </c>
     </row>
@@ -14974,15 +14964,15 @@
         <v>37.051000000000002</v>
       </c>
       <c r="O92">
-        <f>(H92-N92)</f>
+        <f t="shared" si="8"/>
         <v>17.811999999999998</v>
       </c>
       <c r="P92">
-        <f>(E92-N92)</f>
+        <f t="shared" si="9"/>
         <v>10.200299999999999</v>
       </c>
       <c r="Q92">
-        <f>(O92-P92)</f>
+        <f t="shared" si="10"/>
         <v>7.611699999999999</v>
       </c>
     </row>
@@ -15021,15 +15011,15 @@
         <v>37.143000000000001</v>
       </c>
       <c r="O93">
-        <f>(H93-N93)</f>
+        <f t="shared" si="8"/>
         <v>15.427</v>
       </c>
       <c r="P93">
-        <f>(E93-N93)</f>
+        <f t="shared" si="9"/>
         <v>7.7490999999999985</v>
       </c>
       <c r="Q93">
-        <f>(O93-P93)</f>
+        <f t="shared" si="10"/>
         <v>7.6779000000000011</v>
       </c>
       <c r="R93" t="s">
@@ -15062,15 +15052,15 @@
         <v>37.112000000000002</v>
       </c>
       <c r="O94">
-        <f>(H94-N94)</f>
+        <f t="shared" si="8"/>
         <v>19.757999999999996</v>
       </c>
       <c r="P94">
-        <f>(E94-N94)</f>
+        <f t="shared" si="9"/>
         <v>11.444299999999998</v>
       </c>
       <c r="Q94">
-        <f>(O94-P94)</f>
+        <f t="shared" si="10"/>
         <v>8.3136999999999972</v>
       </c>
     </row>
@@ -15100,15 +15090,15 @@
         <v>37.024000000000001</v>
       </c>
       <c r="O95">
-        <f>(H95-N95)</f>
+        <f t="shared" si="8"/>
         <v>17.256</v>
       </c>
       <c r="P95">
-        <f>(E95-N95)</f>
+        <f t="shared" si="9"/>
         <v>8.9309000000000012</v>
       </c>
       <c r="Q95">
-        <f>(O95-P95)</f>
+        <f t="shared" si="10"/>
         <v>8.3250999999999991</v>
       </c>
     </row>
@@ -15156,7 +15146,7 @@
         <v>8.5348199999999963</v>
       </c>
       <c r="Q96">
-        <f>(O96-P96)</f>
+        <f t="shared" si="10"/>
         <v>8.4181799999999996</v>
       </c>
       <c r="R96" t="s">
@@ -15203,7 +15193,7 @@
         <v>11.006509999999999</v>
       </c>
       <c r="Q97">
-        <f>(O97-P97)</f>
+        <f t="shared" si="10"/>
         <v>8.7674900000000022</v>
       </c>
       <c r="R97" t="s">
@@ -15247,7 +15237,7 @@
         <v>10.220399999999998</v>
       </c>
       <c r="Q98">
-        <f>(O98-P98)</f>
+        <f t="shared" ref="Q98:Q129" si="11">(O98-P98)</f>
         <v>9.1114999999999995</v>
       </c>
     </row>
@@ -15285,7 +15275,7 @@
         <v>8.2475000000000023</v>
       </c>
       <c r="Q99">
-        <f>(O99-P99)</f>
+        <f t="shared" si="11"/>
         <v>9.1565999999999974</v>
       </c>
     </row>
@@ -15330,7 +15320,7 @@
         <v>10.921129999999998</v>
       </c>
       <c r="Q100">
-        <f>(O100-P100)</f>
+        <f t="shared" si="11"/>
         <v>9.2078699999999998</v>
       </c>
       <c r="R100" t="s">
@@ -15363,15 +15353,15 @@
         <v>37.222200000000001</v>
       </c>
       <c r="O101">
-        <f>(H101-N101)</f>
+        <f t="shared" ref="O101:O137" si="12">(H101-N101)</f>
         <v>19.084800000000001</v>
       </c>
       <c r="P101">
-        <f>(E101-N101)</f>
+        <f t="shared" ref="P101:P137" si="13">(E101-N101)</f>
         <v>9.873899999999999</v>
       </c>
       <c r="Q101">
-        <f>(O101-P101)</f>
+        <f t="shared" si="11"/>
         <v>9.2109000000000023</v>
       </c>
     </row>
@@ -15401,15 +15391,15 @@
         <v>37.086199999999998</v>
       </c>
       <c r="O102">
-        <f>(H102-N102)</f>
+        <f t="shared" si="12"/>
         <v>20.4938</v>
       </c>
       <c r="P102">
-        <f>(E102-N102)</f>
+        <f t="shared" si="13"/>
         <v>11.160800000000002</v>
       </c>
       <c r="Q102">
-        <f>(O102-P102)</f>
+        <f t="shared" si="11"/>
         <v>9.3329999999999984</v>
       </c>
     </row>
@@ -15439,15 +15429,15 @@
         <v>37.045999999999999</v>
       </c>
       <c r="O103">
-        <f>(H103-N103)</f>
+        <f t="shared" si="12"/>
         <v>21.003999999999998</v>
       </c>
       <c r="P103">
-        <f>(E103-N103)</f>
+        <f t="shared" si="13"/>
         <v>11.644600000000004</v>
       </c>
       <c r="Q103">
-        <f>(O103-P103)</f>
+        <f t="shared" si="11"/>
         <v>9.3593999999999937</v>
       </c>
     </row>
@@ -15477,15 +15467,15 @@
         <v>37.027999999999999</v>
       </c>
       <c r="O104">
-        <f>(H104-N104)</f>
+        <f t="shared" si="12"/>
         <v>25.631999999999998</v>
       </c>
       <c r="P104">
-        <f>(E104-N104)</f>
+        <f t="shared" si="13"/>
         <v>16.230800000000002</v>
       </c>
       <c r="Q104">
-        <f>(O104-P104)</f>
+        <f t="shared" si="11"/>
         <v>9.4011999999999958</v>
       </c>
     </row>
@@ -15515,15 +15505,15 @@
         <v>37.121600000000001</v>
       </c>
       <c r="O105">
-        <f>(H105-N105)</f>
+        <f t="shared" si="12"/>
         <v>22.807400000000001</v>
       </c>
       <c r="P105">
-        <f>(E105-N105)</f>
+        <f t="shared" si="13"/>
         <v>12.883299999999998</v>
       </c>
       <c r="Q105">
-        <f>(O105-P105)</f>
+        <f t="shared" si="11"/>
         <v>9.9241000000000028</v>
       </c>
     </row>
@@ -15553,15 +15543,15 @@
         <v>37.0535</v>
       </c>
       <c r="O106">
-        <f>(H106-N106)</f>
+        <f t="shared" si="12"/>
         <v>24.048499999999997</v>
       </c>
       <c r="P106">
-        <f>(E106-N106)</f>
+        <f t="shared" si="13"/>
         <v>13.789900000000003</v>
       </c>
       <c r="Q106">
-        <f>(O106-P106)</f>
+        <f t="shared" si="11"/>
         <v>10.258599999999994</v>
       </c>
     </row>
@@ -15591,15 +15581,15 @@
         <v>37.098700000000001</v>
       </c>
       <c r="O107">
-        <f>(H107-N107)</f>
+        <f t="shared" si="12"/>
         <v>26.716299999999997</v>
       </c>
       <c r="P107">
-        <f>(E107-N107)</f>
+        <f t="shared" si="13"/>
         <v>15.999699999999997</v>
       </c>
       <c r="Q107">
-        <f>(O107-P107)</f>
+        <f t="shared" si="11"/>
         <v>10.7166</v>
       </c>
     </row>
@@ -15629,15 +15619,15 @@
         <v>37.128799999999998</v>
       </c>
       <c r="O108">
-        <f>(H108-N108)</f>
+        <f t="shared" si="12"/>
         <v>23.441200000000002</v>
       </c>
       <c r="P108">
-        <f>(E108-N108)</f>
+        <f t="shared" si="13"/>
         <v>12.672400000000003</v>
       </c>
       <c r="Q108">
-        <f>(O108-P108)</f>
+        <f t="shared" si="11"/>
         <v>10.768799999999999</v>
       </c>
     </row>
@@ -15667,15 +15657,15 @@
         <v>36.990499999999997</v>
       </c>
       <c r="O109">
-        <f>(H109-N109)</f>
+        <f t="shared" si="12"/>
         <v>25.951500000000003</v>
       </c>
       <c r="P109">
-        <f>(E109-N109)</f>
+        <f t="shared" si="13"/>
         <v>14.973100000000002</v>
       </c>
       <c r="Q109">
-        <f>(O109-P109)</f>
+        <f t="shared" si="11"/>
         <v>10.978400000000001</v>
       </c>
     </row>
@@ -15706,15 +15696,15 @@
         <v>66.219729999999998</v>
       </c>
       <c r="O110">
-        <f>(H110-N110)</f>
+        <f t="shared" si="12"/>
         <v>19.955269999999999</v>
       </c>
       <c r="P110">
-        <f>(E110-N110)</f>
+        <f t="shared" si="13"/>
         <v>8.8997700000000037</v>
       </c>
       <c r="Q110">
-        <f>(O110-P110)</f>
+        <f t="shared" si="11"/>
         <v>11.055499999999995</v>
       </c>
     </row>
@@ -15747,15 +15737,15 @@
         <v>37.139299999999999</v>
       </c>
       <c r="O111">
-        <f>(H111-N111)</f>
+        <f t="shared" si="12"/>
         <v>19.747700000000002</v>
       </c>
       <c r="P111">
-        <f>(E111-N111)</f>
+        <f t="shared" si="13"/>
         <v>8.515500000000003</v>
       </c>
       <c r="Q111">
-        <f>(O111-P111)</f>
+        <f t="shared" si="11"/>
         <v>11.232199999999999</v>
       </c>
       <c r="R111" t="s">
@@ -15789,15 +15779,15 @@
         <v>37.040500000000002</v>
       </c>
       <c r="O112">
-        <f>(H112-N112)</f>
+        <f t="shared" si="12"/>
         <v>20.852499999999999</v>
       </c>
       <c r="P112">
-        <f>(E112-N112)</f>
+        <f t="shared" si="13"/>
         <v>9.4953000000000003</v>
       </c>
       <c r="Q112">
-        <f>(O112-P112)</f>
+        <f t="shared" si="11"/>
         <v>11.357199999999999</v>
       </c>
     </row>
@@ -15827,15 +15817,15 @@
         <v>36.9983</v>
       </c>
       <c r="O113">
-        <f>(H113-N113)</f>
+        <f t="shared" si="12"/>
         <v>23.8827</v>
       </c>
       <c r="P113">
-        <f>(E113-N113)</f>
+        <f t="shared" si="13"/>
         <v>12.483199999999997</v>
       </c>
       <c r="Q113">
-        <f>(O113-P113)</f>
+        <f t="shared" si="11"/>
         <v>11.399500000000003</v>
       </c>
     </row>
@@ -15865,15 +15855,15 @@
         <v>37.005000000000003</v>
       </c>
       <c r="O114">
-        <f>(H114-N114)</f>
+        <f t="shared" si="12"/>
         <v>29.213999999999992</v>
       </c>
       <c r="P114">
-        <f>(E114-N114)</f>
+        <f t="shared" si="13"/>
         <v>17.791799999999995</v>
       </c>
       <c r="Q114">
-        <f>(O114-P114)</f>
+        <f t="shared" si="11"/>
         <v>11.422199999999997</v>
       </c>
     </row>
@@ -15906,15 +15896,15 @@
         <v>37.026800000000001</v>
       </c>
       <c r="O115">
-        <f>(H115-N115)</f>
+        <f t="shared" si="12"/>
         <v>26.912199999999999</v>
       </c>
       <c r="P115">
-        <f>(E115-N115)</f>
+        <f t="shared" si="13"/>
         <v>14.9161</v>
       </c>
       <c r="Q115">
-        <f>(O115-P115)</f>
+        <f t="shared" si="11"/>
         <v>11.996099999999998</v>
       </c>
     </row>
@@ -15944,15 +15934,15 @@
         <v>37.06</v>
       </c>
       <c r="O116">
-        <f>(H116-N116)</f>
+        <f t="shared" si="12"/>
         <v>25.799999999999997</v>
       </c>
       <c r="P116">
-        <f>(E116-N116)</f>
+        <f t="shared" si="13"/>
         <v>13.575299999999999</v>
       </c>
       <c r="Q116">
-        <f>(O116-P116)</f>
+        <f t="shared" si="11"/>
         <v>12.224699999999999</v>
       </c>
     </row>
@@ -15988,15 +15978,15 @@
         <v>37.030999999999999</v>
       </c>
       <c r="O117">
-        <f>(H117-N117)</f>
+        <f t="shared" si="12"/>
         <v>25.122</v>
       </c>
       <c r="P117">
-        <f>(E117-N117)</f>
+        <f t="shared" si="13"/>
         <v>12.805530000000005</v>
       </c>
       <c r="Q117">
-        <f>(O117-P117)</f>
+        <f t="shared" si="11"/>
         <v>12.316469999999995</v>
       </c>
       <c r="R117" t="s">
@@ -16029,15 +16019,15 @@
         <v>37.003700000000002</v>
       </c>
       <c r="O118">
-        <f>(H118-N118)</f>
+        <f t="shared" si="12"/>
         <v>23.996299999999998</v>
       </c>
       <c r="P118">
-        <f>(E118-N118)</f>
+        <f t="shared" si="13"/>
         <v>11.194600000000001</v>
       </c>
       <c r="Q118">
-        <f>(O118-P118)</f>
+        <f t="shared" si="11"/>
         <v>12.801699999999997</v>
       </c>
     </row>
@@ -16067,15 +16057,15 @@
         <v>37.078299999999999</v>
       </c>
       <c r="O119">
-        <f>(H119-N119)</f>
+        <f t="shared" si="12"/>
         <v>27.072699999999998</v>
       </c>
       <c r="P119">
-        <f>(E119-N119)</f>
+        <f t="shared" si="13"/>
         <v>14.259700000000002</v>
       </c>
       <c r="Q119">
-        <f>(O119-P119)</f>
+        <f t="shared" si="11"/>
         <v>12.812999999999995</v>
       </c>
     </row>
@@ -16105,15 +16095,15 @@
         <v>37.158000000000001</v>
       </c>
       <c r="O120">
-        <f>(H120-N120)</f>
+        <f t="shared" si="12"/>
         <v>36.182999999999993</v>
       </c>
       <c r="P120">
-        <f>(E120-N120)</f>
+        <f t="shared" si="13"/>
         <v>21.9236</v>
       </c>
       <c r="Q120">
-        <f>(O120-P120)</f>
+        <f t="shared" si="11"/>
         <v>14.259399999999992</v>
       </c>
     </row>
@@ -16143,15 +16133,15 @@
         <v>37.1464</v>
       </c>
       <c r="O121">
-        <f>(H121-N121)</f>
+        <f t="shared" si="12"/>
         <v>26.373600000000003</v>
       </c>
       <c r="P121">
-        <f>(E121-N121)</f>
+        <f t="shared" si="13"/>
         <v>11.621499999999997</v>
       </c>
       <c r="Q121">
-        <f>(O121-P121)</f>
+        <f t="shared" si="11"/>
         <v>14.752100000000006</v>
       </c>
     </row>
@@ -16181,15 +16171,15 @@
         <v>36.983899999999998</v>
       </c>
       <c r="O122">
-        <f>(H122-N122)</f>
+        <f t="shared" si="12"/>
         <v>31.497099999999996</v>
       </c>
       <c r="P122">
-        <f>(E122-N122)</f>
+        <f t="shared" si="13"/>
         <v>16.629100000000001</v>
       </c>
       <c r="Q122">
-        <f>(O122-P122)</f>
+        <f t="shared" si="11"/>
         <v>14.867999999999995</v>
       </c>
     </row>
@@ -16220,15 +16210,15 @@
         <v>37.010300000000001</v>
       </c>
       <c r="O123">
-        <f>(H123-N123)</f>
+        <f t="shared" si="12"/>
         <v>28.058700000000002</v>
       </c>
       <c r="P123">
-        <f>(E123-N123)</f>
+        <f t="shared" si="13"/>
         <v>12.725099999999998</v>
       </c>
       <c r="Q123">
-        <f>(O123-P123)</f>
+        <f t="shared" si="11"/>
         <v>15.333600000000004</v>
       </c>
     </row>
@@ -16259,15 +16249,15 @@
         <v>36.864199999999997</v>
       </c>
       <c r="O124">
-        <f>(H124-N124)</f>
+        <f t="shared" si="12"/>
         <v>27.94080000000001</v>
       </c>
       <c r="P124">
-        <f>(E124-N124)</f>
+        <f t="shared" si="13"/>
         <v>12.552400000000006</v>
       </c>
       <c r="Q124">
-        <f>(O124-P124)</f>
+        <f t="shared" si="11"/>
         <v>15.388400000000004</v>
       </c>
     </row>
@@ -16297,15 +16287,15 @@
         <v>37.122599999999998</v>
       </c>
       <c r="O125">
-        <f>(H125-N125)</f>
+        <f t="shared" si="12"/>
         <v>29.630400000000002</v>
       </c>
       <c r="P125">
-        <f>(E125-N125)</f>
+        <f t="shared" si="13"/>
         <v>13.672699999999999</v>
       </c>
       <c r="Q125">
-        <f>(O125-P125)</f>
+        <f t="shared" si="11"/>
         <v>15.957700000000003</v>
       </c>
     </row>
@@ -16335,15 +16325,15 @@
         <v>37.0002</v>
       </c>
       <c r="O126">
-        <f>(H126-N126)</f>
+        <f t="shared" si="12"/>
         <v>28.888799999999996</v>
       </c>
       <c r="P126">
-        <f>(E126-N126)</f>
+        <f t="shared" si="13"/>
         <v>12.646700000000003</v>
       </c>
       <c r="Q126">
-        <f>(O126-P126)</f>
+        <f t="shared" si="11"/>
         <v>16.242099999999994</v>
       </c>
     </row>
@@ -16374,15 +16364,15 @@
         <v>36.939599999999999</v>
       </c>
       <c r="O127">
-        <f>(H127-N127)</f>
+        <f t="shared" si="12"/>
         <v>32.6404</v>
       </c>
       <c r="P127">
-        <f>(E127-N127)</f>
+        <f t="shared" si="13"/>
         <v>15.231000000000002</v>
       </c>
       <c r="Q127">
-        <f>(O127-P127)</f>
+        <f t="shared" si="11"/>
         <v>17.409399999999998</v>
       </c>
     </row>
@@ -16412,15 +16402,15 @@
         <v>36.946899999999999</v>
       </c>
       <c r="O128">
-        <f>(H128-N128)</f>
+        <f t="shared" si="12"/>
         <v>37.899100000000004</v>
       </c>
       <c r="P128">
-        <f>(E128-N128)</f>
+        <f t="shared" si="13"/>
         <v>20.142400000000002</v>
       </c>
       <c r="Q128">
-        <f>(O128-P128)</f>
+        <f t="shared" si="11"/>
         <v>17.756700000000002</v>
       </c>
     </row>
@@ -16456,15 +16446,15 @@
         <v>37.107999999999997</v>
       </c>
       <c r="O129">
-        <f>(H129-N129)</f>
+        <f t="shared" si="12"/>
         <v>33.533000000000008</v>
       </c>
       <c r="P129">
-        <f>(E129-N129)</f>
+        <f t="shared" si="13"/>
         <v>14.697100000000006</v>
       </c>
       <c r="Q129">
-        <f>(O129-P129)</f>
+        <f t="shared" si="11"/>
         <v>18.835900000000002</v>
       </c>
       <c r="R129" t="s">
@@ -16503,15 +16493,15 @@
         <v>37.095999999999997</v>
       </c>
       <c r="O130">
-        <f>(H130-N130)</f>
+        <f t="shared" si="12"/>
         <v>33.685000000000009</v>
       </c>
       <c r="P130">
-        <f>(E130-N130)</f>
+        <f t="shared" si="13"/>
         <v>14.465380000000003</v>
       </c>
       <c r="Q130">
-        <f>(O130-P130)</f>
+        <f t="shared" ref="Q130:Q161" si="14">(O130-P130)</f>
         <v>19.219620000000006</v>
       </c>
       <c r="R130" t="s">
@@ -16545,15 +16535,15 @@
         <v>36.8688</v>
       </c>
       <c r="O131">
-        <f>(H131-N131)</f>
+        <f t="shared" si="12"/>
         <v>37.301200000000001</v>
       </c>
       <c r="P131">
-        <f>(E131-N131)</f>
+        <f t="shared" si="13"/>
         <v>15.371499999999997</v>
       </c>
       <c r="Q131">
-        <f>(O131-P131)</f>
+        <f t="shared" si="14"/>
         <v>21.929700000000004</v>
       </c>
     </row>
@@ -16583,15 +16573,15 @@
         <v>36.992600000000003</v>
       </c>
       <c r="O132">
-        <f>(H132-N132)</f>
+        <f t="shared" si="12"/>
         <v>55.372399999999992</v>
       </c>
       <c r="P132">
-        <f>(E132-N132)</f>
+        <f t="shared" si="13"/>
         <v>29.378399999999992</v>
       </c>
       <c r="Q132">
-        <f>(O132-P132)</f>
+        <f t="shared" si="14"/>
         <v>25.994</v>
       </c>
     </row>
@@ -16621,15 +16611,15 @@
         <v>37.106099999999998</v>
       </c>
       <c r="O133">
-        <f>(H133-N133)</f>
+        <f t="shared" si="12"/>
         <v>60.719899999999996</v>
       </c>
       <c r="P133">
-        <f>(E133-N133)</f>
+        <f t="shared" si="13"/>
         <v>30.953900000000004</v>
       </c>
       <c r="Q133">
-        <f>(O133-P133)</f>
+        <f t="shared" si="14"/>
         <v>29.765999999999991</v>
       </c>
     </row>
@@ -16665,15 +16655,15 @@
         <v>37.125999999999998</v>
       </c>
       <c r="O134">
-        <f>(H134-N134)</f>
+        <f t="shared" si="12"/>
         <v>62.051000000000009</v>
       </c>
       <c r="P134">
-        <f>(E134-N134)</f>
+        <f t="shared" si="13"/>
         <v>32.267600000000009</v>
       </c>
       <c r="Q134">
-        <f>(O134-P134)</f>
+        <f t="shared" si="14"/>
         <v>29.7834</v>
       </c>
       <c r="R134" t="s">
@@ -16706,15 +16696,15 @@
         <v>36.956699999999998</v>
       </c>
       <c r="O135">
-        <f>(H135-N135)</f>
+        <f t="shared" si="12"/>
         <v>66.958300000000008</v>
       </c>
       <c r="P135">
-        <f>(E135-N135)</f>
+        <f t="shared" si="13"/>
         <v>34.918300000000002</v>
       </c>
       <c r="Q135">
-        <f>(O135-P135)</f>
+        <f t="shared" si="14"/>
         <v>32.040000000000006</v>
       </c>
     </row>
@@ -16744,15 +16734,15 @@
         <v>36.9313</v>
       </c>
       <c r="O136">
-        <f>(H136-N136)</f>
+        <f t="shared" si="12"/>
         <v>75.421699999999987</v>
       </c>
       <c r="P136">
-        <f>(E136-N136)</f>
+        <f t="shared" si="13"/>
         <v>40.856699999999996</v>
       </c>
       <c r="Q136">
-        <f>(O136-P136)</f>
+        <f t="shared" si="14"/>
         <v>34.564999999999991</v>
       </c>
     </row>
@@ -16789,15 +16779,15 @@
         <v>37.073500000000003</v>
       </c>
       <c r="O137">
-        <f>(H137-N137)</f>
+        <f t="shared" si="12"/>
         <v>2.0625</v>
       </c>
       <c r="P137">
-        <f>(E137-N137)</f>
+        <f t="shared" si="13"/>
         <v>1.0593000000000004</v>
       </c>
       <c r="Q137">
-        <f>(O137-P137)</f>
+        <f t="shared" si="14"/>
         <v>1.0031999999999996</v>
       </c>
     </row>
@@ -16830,19 +16820,19 @@
         <v>116</v>
       </c>
       <c r="N138" s="4">
-        <f t="shared" ref="N138:N143" si="0">AVERAGE(F138,I138)</f>
+        <f t="shared" ref="N138:N143" si="15">AVERAGE(F138,I138)</f>
         <v>37.168500000000002</v>
       </c>
       <c r="O138">
-        <f t="shared" ref="O138:O143" si="1">(H138-N138)</f>
+        <f t="shared" ref="O138:O143" si="16">(H138-N138)</f>
         <v>18.008499999999998</v>
       </c>
       <c r="P138">
-        <f t="shared" ref="P138:P143" si="2">(E138-N138)</f>
+        <f t="shared" ref="P138:P143" si="17">(E138-N138)</f>
         <v>9.7560000000000002</v>
       </c>
       <c r="Q138">
-        <f t="shared" ref="Q138:Q143" si="3">(O138-P138)</f>
+        <f t="shared" ref="Q138:Q143" si="18">(O138-P138)</f>
         <v>8.2524999999999977</v>
       </c>
     </row>
@@ -16875,19 +16865,19 @@
         <v>116</v>
       </c>
       <c r="N139" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="15"/>
         <v>37.057000000000002</v>
       </c>
       <c r="O139">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>19.800999999999995</v>
       </c>
       <c r="P139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>10.458079999999995</v>
       </c>
       <c r="Q139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>9.3429199999999994</v>
       </c>
     </row>
@@ -16920,19 +16910,19 @@
         <v>116</v>
       </c>
       <c r="N140" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="15"/>
         <v>37.155999999999999</v>
       </c>
       <c r="O140">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>23.289000000000001</v>
       </c>
       <c r="P140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>11.615099999999998</v>
       </c>
       <c r="Q140">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>11.673900000000003</v>
       </c>
     </row>
@@ -16965,19 +16955,19 @@
         <v>116</v>
       </c>
       <c r="N141" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="15"/>
         <v>37.072499999999998</v>
       </c>
       <c r="O141">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>17.419499999999999</v>
       </c>
       <c r="P141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>8.991500000000002</v>
       </c>
       <c r="Q141">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>8.4279999999999973</v>
       </c>
     </row>
@@ -17010,19 +17000,19 @@
         <v>116</v>
       </c>
       <c r="N142" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="15"/>
         <v>37.067</v>
       </c>
       <c r="O142">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>20.310000000000002</v>
       </c>
       <c r="P142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>9.5260999999999996</v>
       </c>
       <c r="Q142">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>10.783900000000003</v>
       </c>
     </row>
@@ -17055,19 +17045,19 @@
         <v>116</v>
       </c>
       <c r="N143" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="15"/>
         <v>37.087500000000006</v>
       </c>
       <c r="O143">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>20.735499999999995</v>
       </c>
       <c r="P143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>9.5424999999999969</v>
       </c>
       <c r="Q143">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>11.192999999999998</v>
       </c>
     </row>
@@ -17083,14 +17073,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5750438-5322-5A46-95A8-63380D05FED0}">
   <dimension ref="A1:R143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="16" width="11" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
+    <col min="18" max="18" width="11" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>